<commit_message>
Added a line of code to convert all values to float after being added to dataframe. This will ensure all figures have 2 decimal places when later code is executed
</commit_message>
<xml_diff>
--- a/New Sheet.xlsx
+++ b/New Sheet.xlsx
@@ -458,10 +458,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">All </t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>99</v>
       </c>
     </row>
@@ -471,7 +471,7 @@
           <t>Joe L</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -481,7 +481,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -491,7 +491,7 @@
           <t>Michael B</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>847.86</v>
+        <v>809.75</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -572,7 +572,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11870.04</v>
+        <v>11336.5</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -581,7 +581,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7838.04</v>
+        <v>7304.5</v>
       </c>
     </row>
     <row r="3">
@@ -591,14 +591,16 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1232.54</v>
+        <v>1196.54</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" s="2" t="n">
-        <v>6162.7</v>
+        <v>5982.7</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>2394</v>
@@ -607,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>3768.7</v>
+        <v>3588.7</v>
       </c>
     </row>
     <row r="4">
@@ -617,7 +619,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>221.07</v>
+        <v>215.52</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>3</v>
@@ -626,7 +628,7 @@
         <v>2750</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>663.21</v>
+        <v>646.5599999999999</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>178.26</v>
@@ -635,7 +637,7 @@
         <v>2452.9</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>484.95</v>
+        <v>468.3</v>
       </c>
     </row>
     <row r="5">
@@ -645,14 +647,16 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>26.21</v>
+        <v>26.44</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E5" s="2" t="n">
-        <v>131.05</v>
+        <v>132.2</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>107.6</v>
@@ -661,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>23.45</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="6">
@@ -671,14 +675,16 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>34.98</v>
+        <v>34.53</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E6" s="2" t="n">
-        <v>524.7</v>
+        <v>517.95</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>799.65</v>
@@ -687,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>-274.95</v>
+        <v>-281.7</v>
       </c>
     </row>
     <row r="7">
@@ -697,14 +703,16 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>138.99</v>
+        <v>142.45</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E7" s="2" t="n">
-        <v>1667.88</v>
+        <v>1709.4</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1680.6</v>
@@ -713,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>-12.72</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="8">
@@ -723,14 +731,16 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>154.53</v>
+        <v>148.07</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" s="2" t="n">
-        <v>772.65</v>
+        <v>740.35</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>775</v>
@@ -739,7 +749,35 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>-2.35</v>
+        <v>-34.65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>334.53</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>4014.36</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>4000.68</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>13.68</v>
       </c>
     </row>
   </sheetData>
@@ -753,7 +791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,7 +847,7 @@
           <t>Joe L</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="n">
@@ -825,7 +863,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>15</v>
       </c>
       <c r="G2" s="2" t="n">
@@ -841,7 +879,7 @@
           <t>Joe L</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="n">
@@ -857,14 +895,14 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="2" t="n">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>53.31</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>799.6500000000001</v>
+        <v>799.65</v>
       </c>
     </row>
     <row r="4">
@@ -873,7 +911,7 @@
           <t>Joe L</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
@@ -889,7 +927,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="n">
@@ -905,7 +943,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -921,7 +959,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="2" t="n">
         <v>8</v>
       </c>
       <c r="G5" s="2" t="n">
@@ -937,7 +975,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -953,7 +991,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -969,7 +1007,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="n">
@@ -985,7 +1023,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="2" t="n">
         <v>12</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -1001,7 +1039,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -1017,7 +1055,7 @@
           <t>Sell</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="n">
@@ -1033,7 +1071,7 @@
           <t>Jonathan R</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="n">
@@ -1049,7 +1087,7 @@
           <t>Sell</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G9" s="2" t="n">
@@ -1065,7 +1103,7 @@
           <t>Michael B</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="2" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="n">
@@ -1081,7 +1119,7 @@
           <t>Buy</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="n">
@@ -1089,6 +1127,38 @@
       </c>
       <c r="H10" s="2" t="n">
         <v>775</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>333.39</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>4000.68</v>
       </c>
     </row>
   </sheetData>
@@ -1161,7 +1231,7 @@
       <c r="B2" s="2" t="n">
         <v>844.54</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="n">
@@ -1189,10 +1259,12 @@
       <c r="B3" s="2" t="n">
         <v>1228</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" s="2" t="n">
         <v>6140</v>
       </c>
@@ -1215,10 +1287,12 @@
       <c r="B4" s="2" t="n">
         <v>34.94</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E4" s="2" t="n">
         <v>524.1</v>
       </c>
@@ -1302,7 +1376,7 @@
       <c r="B2" s="2" t="n">
         <v>844.54</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>14</v>
       </c>
       <c r="D2" s="2" t="n">
@@ -1330,7 +1404,7 @@
       <c r="B3" s="2" t="n">
         <v>219.8</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -1358,10 +1432,12 @@
       <c r="B4" s="2" t="n">
         <v>26.21</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E4" s="2" t="n">
         <v>131.05</v>
       </c>
@@ -1384,10 +1460,12 @@
       <c r="B5" s="2" t="n">
         <v>138.51</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E5" s="2" t="n">
         <v>1662.12</v>
       </c>
@@ -1468,23 +1546,25 @@
           <t>AMD</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>154</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>770</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>775</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issue where new transactions weren't being listed on investor pages.
</commit_message>
<xml_diff>
--- a/New Sheet.xlsx
+++ b/New Sheet.xlsx
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,113 +559,113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>809.75</v>
+        <v>149.58</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>870.45</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11336.5</v>
+        <v>747.9</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>4032</v>
+        <v>775</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>582.45</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7304.5</v>
+        <v>-27.1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MSTR</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1196.54</v>
+        <v>335.18</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>5982.7</v>
+        <v>4022.16</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2394</v>
+        <v>4000.68</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>3588.7</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>COIN</t>
+          <t>NFLX</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>215.52</v>
+        <v>556.13</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2750</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>646.5599999999999</v>
+        <v>2780.65</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>178.26</v>
+        <v>2785.95</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>2452.9</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>468.3</v>
+        <v>-5.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CCOR</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>26.44</v>
+        <v>810.7</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0</v>
+        <v>870.45</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>132.2</v>
+        <v>11349.8</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>107.6</v>
+        <v>4032</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0</v>
+        <v>582.45</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>24.6</v>
+        <v>7317.8</v>
       </c>
     </row>
     <row r="6">
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>34.53</v>
+        <v>34.78</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>15</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>517.95</v>
+        <v>521.7</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>799.65</v>
@@ -693,91 +693,119 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>-281.7</v>
+        <v>-277.95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MTB</t>
+          <t>MSTR</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>142.45</v>
+        <v>1213.82</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1709.4</v>
+        <v>6069.1</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>1680.6</v>
+        <v>2394</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>28.8</v>
+        <v>3675.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>COIN</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>148.07</v>
+        <v>216.95</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>2750</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>740.35</v>
+        <v>650.85</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>775</v>
+        <v>178.26</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0</v>
+        <v>2452.9</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>-34.65</v>
+        <v>472.59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>CCOR</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>334.53</v>
+        <v>26.41</v>
       </c>
       <c r="C9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>107.6</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>24.45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MTB</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>142.44</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>4014.36</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>4000.68</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>13.68</v>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1709.28</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>1680.6</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>28.68</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,7 +830,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Investor</t>
+          <t>Individual</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1159,6 +1187,38 @@
       </c>
       <c r="H11" s="2" t="n">
         <v>4000.68</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>557.1900000000001</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>2785.95</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1289,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>844.54</v>
+        <v>810.7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1238,7 +1298,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11823.56</v>
+        <v>11349.8</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1247,63 +1307,63 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7791.56</v>
+        <v>7317.8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MSTR</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1228</v>
+        <v>34.78</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>6140</v>
+        <v>521.7</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2394</v>
+        <v>799.65</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>3746</v>
+        <v>-277.95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>MSTR</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>34.94</v>
+        <v>1213.82</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>524.1</v>
+        <v>6069.1</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>799.65</v>
+        <v>2394</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-275.55</v>
+        <v>3675.1</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1434,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>844.54</v>
+        <v>810.7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1383,7 +1443,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11823.56</v>
+        <v>11349.8</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1392,7 +1452,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7791.56</v>
+        <v>7317.8</v>
       </c>
     </row>
     <row r="3">
@@ -1402,7 +1462,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>219.8</v>
+        <v>216.95</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3</v>
@@ -1411,7 +1471,7 @@
         <v>2750</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>659.4</v>
+        <v>650.85</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>178.26</v>
@@ -1420,7 +1480,7 @@
         <v>2452.9</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>481.14</v>
+        <v>472.59</v>
       </c>
     </row>
     <row r="4">
@@ -1430,7 +1490,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>26.21</v>
+        <v>26.41</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1439,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>131.05</v>
+        <v>132.05</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>107.6</v>
@@ -1448,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>23.45</v>
+        <v>24.45</v>
       </c>
     </row>
     <row r="5">
@@ -1458,7 +1518,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>138.51</v>
+        <v>142.44</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>12</v>
@@ -1467,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1662.12</v>
+        <v>1709.28</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>1680.6</v>
@@ -1476,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>-18.48</v>
+        <v>28.68</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1547,7 +1607,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>154</v>
+        <v>149.58</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>5</v>
@@ -1556,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>770</v>
+        <v>747.9</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>775</v>
@@ -1565,7 +1625,63 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-5</v>
+        <v>-27.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>335.18</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>4022.16</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>4000.68</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>21.48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>556.13</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>2780.65</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>2785.95</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>-5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated App to properly copy transactions to investors individual sheets Reverted code on streamlit app to keep "All" on streamlit
</commit_message>
<xml_diff>
--- a/New Sheet.xlsx
+++ b/New Sheet.xlsx
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Joe L" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jonathan R" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Michael B" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,7 +459,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Summary</t>
+          <t>All</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -506,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +564,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>149.58</v>
+        <v>149.52</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>5</v>
@@ -572,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>747.9</v>
+        <v>747.6</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>775</v>
@@ -581,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-27.1</v>
+        <v>-27.4</v>
       </c>
     </row>
     <row r="3">
@@ -591,7 +592,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>335.18</v>
+        <v>334.56</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>12</v>
@@ -600,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4022.16</v>
+        <v>4014.72</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>4000.68</v>
@@ -609,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>21.48</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="4">
@@ -619,7 +620,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>556.13</v>
+        <v>557.33</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -628,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2780.65</v>
+        <v>2786.65</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2785.95</v>
@@ -637,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-5.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -647,7 +648,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>810.7</v>
+        <v>804.08</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>14</v>
@@ -656,7 +657,7 @@
         <v>870.45</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>11349.8</v>
+        <v>11257.12</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>4032</v>
@@ -665,7 +666,7 @@
         <v>582.45</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>7317.8</v>
+        <v>7225.12</v>
       </c>
     </row>
     <row r="6">
@@ -675,7 +676,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>34.78</v>
+        <v>34.71</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>15</v>
@@ -684,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>521.7</v>
+        <v>520.65</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>799.65</v>
@@ -693,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>-277.95</v>
+        <v>-279</v>
       </c>
     </row>
     <row r="7">
@@ -703,7 +704,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1213.82</v>
+        <v>1206.99</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>5</v>
@@ -712,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>6069.1</v>
+        <v>6034.95</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>2394</v>
@@ -721,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>3675.1</v>
+        <v>3640.95</v>
       </c>
     </row>
     <row r="8">
@@ -731,7 +732,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>216.95</v>
+        <v>217.1</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>3</v>
@@ -740,7 +741,7 @@
         <v>2750</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>650.85</v>
+        <v>651.3</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>178.26</v>
@@ -749,7 +750,7 @@
         <v>2452.9</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>472.59</v>
+        <v>473.04</v>
       </c>
     </row>
     <row r="9">
@@ -787,7 +788,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>142.44</v>
+        <v>142.46</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>12</v>
@@ -796,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1709.28</v>
+        <v>1709.52</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1680.6</v>
@@ -805,7 +806,35 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>28.68</v>
+        <v>28.92</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>175.96</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>175.96</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>185</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>-9.039999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,7 +859,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Individual</t>
+          <t>Investor</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1219,6 +1248,38 @@
       </c>
       <c r="H12" s="2" t="n">
         <v>2785.95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>185</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1350,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>810.7</v>
+        <v>804.08</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1298,7 +1359,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11349.8</v>
+        <v>11257.12</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1307,7 +1368,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7317.8</v>
+        <v>7225.12</v>
       </c>
     </row>
     <row r="3">
@@ -1317,7 +1378,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>34.78</v>
+        <v>34.71</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -1326,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>521.7</v>
+        <v>520.65</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>799.65</v>
@@ -1335,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>-277.95</v>
+        <v>-279</v>
       </c>
     </row>
     <row r="4">
@@ -1345,7 +1406,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1213.82</v>
+        <v>1206.99</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1354,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6069.1</v>
+        <v>6034.95</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2394</v>
@@ -1363,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3675.1</v>
+        <v>3640.95</v>
       </c>
     </row>
   </sheetData>
@@ -1434,7 +1495,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>810.7</v>
+        <v>804.08</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1443,7 +1504,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11349.8</v>
+        <v>11257.12</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1452,7 +1513,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7317.8</v>
+        <v>7225.12</v>
       </c>
     </row>
     <row r="3">
@@ -1462,7 +1523,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>216.95</v>
+        <v>217.1</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3</v>
@@ -1471,7 +1532,7 @@
         <v>2750</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>650.85</v>
+        <v>651.3</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>178.26</v>
@@ -1480,7 +1541,7 @@
         <v>2452.9</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>472.59</v>
+        <v>473.04</v>
       </c>
     </row>
     <row r="4">
@@ -1518,7 +1579,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>142.44</v>
+        <v>142.46</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>12</v>
@@ -1527,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1709.28</v>
+        <v>1709.52</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>1680.6</v>
@@ -1536,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>28.68</v>
+        <v>28.92</v>
       </c>
     </row>
   </sheetData>
@@ -1550,7 +1611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1607,7 +1668,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>149.58</v>
+        <v>149.52</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>5</v>
@@ -1616,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>747.9</v>
+        <v>747.6</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>775</v>
@@ -1625,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-27.1</v>
+        <v>-27.4</v>
       </c>
     </row>
     <row r="3">
@@ -1635,7 +1696,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>335.18</v>
+        <v>334.56</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>12</v>
@@ -1644,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4022.16</v>
+        <v>4014.72</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>4000.68</v>
@@ -1653,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>21.48</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="4">
@@ -1663,7 +1724,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>556.13</v>
+        <v>557.33</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1672,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2780.65</v>
+        <v>2786.65</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2785.95</v>
@@ -1681,7 +1742,96 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>-5.3</v>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>175.96</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>175.96</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>185</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>-9.039999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price Today</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Realized Sales</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Current Value</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cost Basis</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Realized Profit</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unrealized Profit</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed redundant code that was affecting the cost basis calculation
</commit_message>
<xml_diff>
--- a/New Sheet.xlsx
+++ b/New Sheet.xlsx
@@ -560,67 +560,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AMD</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>149.52</v>
+        <v>762</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>747.6</v>
+        <v>10668</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>775</v>
+        <v>4032</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0</v>
+        <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-27.4</v>
+        <v>6636</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>334.56</v>
+        <v>34.2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4014.72</v>
+        <v>513</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>4000.68</v>
+        <v>799.65</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>14.04</v>
+        <v>-286.65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>MSTR</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>557.33</v>
+        <v>1174.11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -629,184 +629,184 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2786.65</v>
+        <v>5870.55</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>2785.95</v>
+        <v>2394</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.7</v>
+        <v>3476.55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>COIN</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>804.08</v>
+        <v>211.01</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>870.45</v>
+        <v>2750</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>11257.12</v>
+        <v>633.03</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>4032</v>
+        <v>178.26</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>582.45</v>
+        <v>2452.9</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>7225.12</v>
+        <v>454.77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>CCOR</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>34.71</v>
+        <v>26.46</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>520.65</v>
+        <v>132.3</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>799.65</v>
+        <v>107.6</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>-279</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MSTR</t>
+          <t>MTB</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1206.99</v>
+        <v>143.38</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>6034.95</v>
+        <v>1720.56</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>2394</v>
+        <v>1680.6</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>3640.95</v>
+        <v>39.96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>COIN</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>217.1</v>
+        <v>146.64</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2750</v>
+        <v>1310</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>651.3</v>
+        <v>439.92</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>178.26</v>
+        <v>155</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>2452.9</v>
+        <v>690</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>473.04</v>
+        <v>284.92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CCOR</t>
+          <t>HD</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>26.41</v>
+        <v>335.36</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>132.05</v>
+        <v>4024.32</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>107.6</v>
+        <v>4000.68</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>24.45</v>
+        <v>23.64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MTB</t>
+          <t>NFLX</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>142.46</v>
+        <v>555.04</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1709.52</v>
+        <v>2775.2</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1680.6</v>
+        <v>2785.95</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>28.92</v>
+        <v>-10.75</v>
       </c>
     </row>
     <row r="11">
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>175.96</v>
+        <v>175.77</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1</v>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>175.96</v>
+        <v>175.77</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>185</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>-9.039999999999999</v>
+        <v>-9.23</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1164,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>45399</v>
+        <v>45398</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1196,26 +1196,26 @@
         <v>3</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>45401</v>
+        <v>45399</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>333.39</v>
+        <v>155</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>4000.68</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12">
@@ -1228,26 +1228,26 @@
         <v>3</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>45401</v>
+        <v>45399</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>NFLX</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>557.1900000000001</v>
+        <v>500</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>2785.95</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13">
@@ -1260,25 +1260,121 @@
         <v>3</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>45401</v>
+        <v>45400</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>SAP</t>
+          <t>AMD</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="F13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>333.39</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>4000.68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>NFLX</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>557.1900000000001</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>2785.95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Michael B</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>45401</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SAP</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="n">
         <v>185</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H16" s="2" t="n">
         <v>185</v>
       </c>
     </row>
@@ -1350,7 +1446,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>804.08</v>
+        <v>762</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1359,7 +1455,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11257.12</v>
+        <v>10668</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1368,7 +1464,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7225.12</v>
+        <v>6636</v>
       </c>
     </row>
     <row r="3">
@@ -1378,7 +1474,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>34.71</v>
+        <v>34.2</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>15</v>
@@ -1387,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>520.65</v>
+        <v>513</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>799.65</v>
@@ -1396,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>-279</v>
+        <v>-286.65</v>
       </c>
     </row>
     <row r="4">
@@ -1406,7 +1502,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1206.99</v>
+        <v>1174.11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1415,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6034.95</v>
+        <v>5870.55</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2394</v>
@@ -1424,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3640.95</v>
+        <v>3476.55</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1591,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>804.08</v>
+        <v>762</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>14</v>
@@ -1504,7 +1600,7 @@
         <v>870.45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>11257.12</v>
+        <v>10668</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>4032</v>
@@ -1513,7 +1609,7 @@
         <v>582.45</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>7225.12</v>
+        <v>6636</v>
       </c>
     </row>
     <row r="3">
@@ -1523,7 +1619,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>217.1</v>
+        <v>211.01</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3</v>
@@ -1532,7 +1628,7 @@
         <v>2750</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>651.3</v>
+        <v>633.03</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>178.26</v>
@@ -1541,7 +1637,7 @@
         <v>2452.9</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>473.04</v>
+        <v>454.77</v>
       </c>
     </row>
     <row r="4">
@@ -1551,7 +1647,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>26.41</v>
+        <v>26.46</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1560,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>132.05</v>
+        <v>132.3</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>107.6</v>
@@ -1569,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>24.45</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="5">
@@ -1579,7 +1675,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>142.46</v>
+        <v>143.38</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>12</v>
@@ -1588,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1709.52</v>
+        <v>1720.56</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>1680.6</v>
@@ -1597,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>28.92</v>
+        <v>39.96</v>
       </c>
     </row>
   </sheetData>
@@ -1668,25 +1764,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>149.52</v>
+        <v>146.64</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>1310</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>747.6</v>
+        <v>439.92</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>775</v>
+        <v>155</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0</v>
+        <v>690</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>-27.4</v>
+        <v>284.92</v>
       </c>
     </row>
     <row r="3">
@@ -1696,7 +1792,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>334.56</v>
+        <v>335.36</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>12</v>
@@ -1705,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4014.72</v>
+        <v>4024.32</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>4000.68</v>
@@ -1714,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>14.04</v>
+        <v>23.64</v>
       </c>
     </row>
     <row r="4">
@@ -1724,7 +1820,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>557.33</v>
+        <v>555.04</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -1733,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2786.65</v>
+        <v>2775.2</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>2785.95</v>
@@ -1742,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.7</v>
+        <v>-10.75</v>
       </c>
     </row>
     <row r="5">
@@ -1752,7 +1848,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>175.96</v>
+        <v>175.77</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -1761,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>175.96</v>
+        <v>175.77</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>185</v>
@@ -1770,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>-9.039999999999999</v>
+        <v>-9.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed error where Unrealized Profit would be equal to Price Today when quantity is 0
</commit_message>
<xml_diff>
--- a/New Sheet.xlsx
+++ b/New Sheet.xlsx
@@ -735,22 +735,22 @@
         <v>146.64</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>1310</v>
+        <v>1465</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>439.92</v>
+        <v>146.64</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>690</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>284.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1273,13 @@
         </is>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>155</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>155</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14">
@@ -1767,22 +1767,22 @@
         <v>146.64</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1310</v>
+        <v>1465</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>439.92</v>
+        <v>146.64</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>690</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>284.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>